<commit_message>
Added an excel document with graphs of the PID exprimental results. Updated BOM with missing components.
</commit_message>
<xml_diff>
--- a/Circuit Design/BOM.xlsx
+++ b/Circuit Design/BOM.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t>Item Description</t>
   </si>
@@ -36,9 +37,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://www.amazon.co.uk/gp/product/B00650P2ZC/ref=ox_sc_sfl_title_1?ie=UTF8&amp;psc=1&amp;smid=A38F5RZ72I2JQ</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -99,9 +97,6 @@
     <t>39-01-2020</t>
   </si>
   <si>
-    <t>Crimp</t>
-  </si>
-  <si>
     <t>Mini-fit Jr Crimp</t>
   </si>
   <si>
@@ -114,9 +109,6 @@
     <t>WM4330-ND</t>
   </si>
   <si>
-    <t>https://www.digikey.co.uk/products/en?keywords=0470531000</t>
-  </si>
-  <si>
     <t>WM1114-ND</t>
   </si>
   <si>
@@ -291,24 +283,6 @@
     <t>https://uk.rs-online.com/web/p/general-purpose-enclosures/8180457/</t>
   </si>
   <si>
-    <t>50W Heating Element</t>
-  </si>
-  <si>
-    <t>DBK Enclosures</t>
-  </si>
-  <si>
-    <t>HPG-1.5/11-40X35-12-30</t>
-  </si>
-  <si>
-    <t>725-6480 </t>
-  </si>
-  <si>
-    <t>https://uk.rs-online.com/web/p/enclosure-heating-elements/7256480/</t>
-  </si>
-  <si>
-    <t>Total Orders:</t>
-  </si>
-  <si>
     <t>12 V 150 W Heater </t>
   </si>
   <si>
@@ -318,32 +292,79 @@
     <t>B01N0Q9RQ4</t>
   </si>
   <si>
-    <t>https://www.amazon.co.uk/Adhere-Fly-Aluminum-Thermostat-Temperature/dp/B01N0Q9RQ4/ref=pd_day0_107_9?_encoding=UTF8&amp;psc=1&amp;refRID=QCTZEQQF5RFKNGRZ3H98</t>
-  </si>
-  <si>
     <t>670-6307 </t>
   </si>
   <si>
-    <t>https://uk.rs-online.com/web/p/pcb-connector-contacts/6706307/?searchTerm=39-00-0038&amp;relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D656E266D6D3D6D61746368616C6C7061727469616C26706D3D5E2E2A2426706F3D31333326736E3D592673743D43415443485F414C4C5F44454641554C542673633D592677633D4E4F4E45267573743D33392D30302D30303338267374613D33392D30302D3030333826</t>
-  </si>
-  <si>
     <t>484-1748</t>
   </si>
   <si>
-    <t>https://uk.rs-online.com/web/p/pcb-connector-housings/4841748/?searchTerm=39-01-2020&amp;relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D656E266D6D3D6D61746368616C6C7061727469616C26706D3D5E2E2A2426706F3D31333326736E3D592673743D43415443485F414C4C5F44454641554C542673633D592677633D4E4F4E45267573743D33392D30312D32303230267374613D33392D30312D3230323026</t>
+    <t>Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rasberry Pi 3 </t>
+  </si>
+  <si>
+    <t>Model B</t>
+  </si>
+  <si>
+    <t>B01CD5VC92</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Raspberry-Pi-Model-Quad-Motherboard/dp/B01CD5VC92</t>
+  </si>
+  <si>
+    <t>B00U8THDR6</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Elastic-Smooth-Durable-Quality-Metres/dp/B00U8THDR6</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-housings/4841748/</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-connector-contacts/6706307/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Adhere-Fly-Aluminum-Thermostat-Temperature/dp/B01N0Q9RQ4</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/0470531000/WM4330-ND/2421261</t>
+  </si>
+  <si>
+    <t>ELA25-0721BLK</t>
+  </si>
+  <si>
+    <t>The Cut &amp; Sew Comp.</t>
+  </si>
+  <si>
+    <t>Additionally required :</t>
+  </si>
+  <si>
+    <t>Selection of Wires</t>
+  </si>
+  <si>
+    <t>Monitor &amp; Keyboard</t>
+  </si>
+  <si>
+    <t>Selections of Screws &amp; Spacers</t>
+  </si>
+  <si>
+    <t>Standard Crimps</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Noctua-NF-F12PWM-Case-Fan-120/dp/B00650P2ZC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.000;[Red]\-&quot;£&quot;#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +385,26 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -392,7 +433,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -415,11 +456,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -451,17 +518,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,18 +842,18 @@
   <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="164.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="119.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -770,32 +861,40 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="21">
-        <f>10.66+17.49+7.69+42.25</f>
-        <v>78.09</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="33"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="20" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="35"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
+      <c r="F4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="13"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -803,19 +902,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>1</v>
@@ -834,206 +933,212 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="26">
         <v>1</v>
       </c>
-      <c r="B8" s="7">
-        <v>17.489999999999998</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" s="22">
+        <v>32.950000000000003</v>
+      </c>
+      <c r="C8" s="22">
         <f t="shared" ref="C8:C28" si="0">A8*B8</f>
-        <v>17.489999999999998</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="10" t="s">
+        <v>32.950000000000003</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>5</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="7">
-        <v>3.98</v>
+        <v>17.489999999999998</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" si="0"/>
-        <v>7.96</v>
+        <v>17.489999999999998</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="10" t="s">
         <v>16</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="7">
-        <v>7</v>
+        <v>3.98</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>7.96</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>1</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="7">
+        <v>7</v>
+      </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="8"/>
+        <v>80</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="13">
+        <v>10870</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="H11" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="11">
         <v>1</v>
       </c>
       <c r="B12" s="7">
-        <v>21.49</v>
+        <v>1.71</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
+        <v>1.71</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7">
         <v>21.49</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>21.49</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="I13" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="8" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>1</v>
+      </c>
+      <c r="B14" s="22">
+        <v>6.14</v>
+      </c>
+      <c r="C14" s="22">
+        <v>6.14</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="E14" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="F14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="24" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
-        <v>1</v>
-      </c>
-      <c r="B13" s="23">
-        <v>6.14</v>
-      </c>
-      <c r="C13" s="23">
-        <v>6.14</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" s="26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7">
-        <v>10.38</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="0"/>
-        <v>20.76</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>94</v>
+      <c r="I14" s="25" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1048,29 +1153,29 @@
         <v>0.72</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="H15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>2</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>0.19800000000000001</v>
       </c>
       <c r="C16" s="7">
@@ -1078,29 +1183,29 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>4</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="21">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="C17" s="7">
@@ -1108,22 +1213,22 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1138,22 +1243,22 @@
         <v>0.3</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" s="13">
         <v>470531000</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1168,22 +1273,22 @@
         <v>1.65</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="H19" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1198,22 +1303,22 @@
         <v>0.32</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" s="15">
         <v>22232031</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1228,22 +1333,22 @@
         <v>0.24</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="13">
         <v>22012037</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1258,22 +1363,22 @@
         <v>0.54</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F22" s="13">
         <v>39281043</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,22 +1393,22 @@
         <v>0.37</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1318,22 +1423,22 @@
         <v>0.42</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="I24" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,22 +1453,22 @@
         <v>0.22</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="H25" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1378,22 +1483,22 @@
         <v>0.18</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="H26" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1408,22 +1513,22 @@
         <v>0.68</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="I27" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1438,22 +1543,22 @@
         <v>2.34</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="I28" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1463,27 +1568,27 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C30" s="7">
-        <f>SUM(C8:C28)</f>
-        <v>89.364000000000019</v>
-      </c>
-      <c r="H30" s="3"/>
+        <f>SUM(C9:C28)</f>
+        <v>70.314000000000021</v>
+      </c>
+      <c r="H30" s="30"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H31" s="3"/>
+      <c r="H31" s="29"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F32" s="5"/>
-      <c r="H32" s="3"/>
+      <c r="H32" s="28"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33" s="19"/>
-      <c r="H33" s="3"/>
+      <c r="H33" s="27"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
@@ -2050,6 +2155,10 @@
       <c r="I217" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>